<commit_message>
arkitektur og kravsscenerier tilføjet
</commit_message>
<xml_diff>
--- a/Rapport/includes/risikoanalyse.xlsx
+++ b/Rapport/includes/risikoanalyse.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>25.11.2013</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Emulator viser ikke rigtige resultat</t>
@@ -469,7 +466,7 @@
   <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -509,15 +506,17 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
         <v>7</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2">
+        <v>21</v>
+      </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8">
@@ -528,16 +527,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2">
         <v>8</v>
       </c>
       <c r="G4" s="2">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -549,15 +548,17 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
         <v>8</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>64</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8">
@@ -568,7 +569,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
         <v>5</v>
@@ -589,15 +590,17 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>25</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8">
@@ -608,7 +611,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
         <v>8</v>
@@ -616,7 +619,9 @@
       <c r="F8" s="2">
         <v>10</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2">
+        <v>80</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8">
@@ -627,15 +632,17 @@
         <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2">
         <v>6</v>
       </c>
       <c r="F9" s="2">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="2">
+        <v>36</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:8">
@@ -646,15 +653,17 @@
         <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>27</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8">
@@ -665,15 +674,17 @@
         <v>6</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2">
         <v>10</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>20</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8">
@@ -684,13 +695,17 @@
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>40</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="2:8">
@@ -701,11 +716,17 @@
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2">
+        <v>24</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8">
@@ -716,11 +737,17 @@
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E14" s="2">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>30</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8">

</xml_diff>